<commit_message>
update mâu kế hoạch năm
</commit_message>
<xml_diff>
--- a/assets/template/year2.xlsx
+++ b/assets/template/year2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\qc\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4E154D-6C49-4073-AF9B-0F323CAFB517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7F055F-560D-4CBF-9528-EE5D31CB8EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -207,7 +207,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -237,6 +237,43 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -267,28 +304,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,9 +658,8 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B22" sqref="B22"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -632,36 +668,36 @@
     <col min="2" max="2" width="21.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="7" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="15" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" s="7" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -669,24 +705,24 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -704,229 +740,230 @@
       <c r="E3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" s="8" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-    </row>
-    <row r="5" spans="1:23" s="8" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-    </row>
-    <row r="6" spans="1:23" s="9" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-    </row>
-    <row r="7" spans="1:23" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+    </row>
+    <row r="5" spans="1:23" s="8" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+    </row>
+    <row r="6" spans="1:23" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E6" s="5">
         <v>2101010011</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+    </row>
+    <row r="7" spans="1:23" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
     </row>
     <row r="8" spans="1:23" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
     </row>
     <row r="9" spans="1:23" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
     </row>
     <row r="10" spans="1:23" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
     </row>
     <row r="11" spans="1:23" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
     </row>
     <row r="12" spans="1:23" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
     <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="E3:E5"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.25" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>
+  <pageMargins left="0.51181102362204722" right="0.23622047244094491" top="0.51181102362204722" bottom="0.51181102362204722" header="0.23622047244094491" footer="0.23622047244094491"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;C&amp;12
 </oddHeader>
-    <oddFooter>&amp;L&amp;12Mã số phụ lục / &amp;"Times New Roman,Italic"Appendix No.&amp;"Times New Roman,Regular" 0002020_A02_01&amp;C&amp;12Ngày hiệu lực / &amp;"Times New Roman,Italic"Appendix effective&amp;"Times New Roman,Regular" 29/05/2023&amp;R&amp;12Trang / Page &amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;12Mã số phụ lục / &amp;"Times New Roman,Italic"Appendix No.&amp;"Times New Roman,Regular" 0002020_A02_02&amp;C&amp;12Ngày hiệu lực / &amp;"Times New Roman,Italic"Appendix effective&amp;"Times New Roman,Regular" 18/01/2024&amp;R&amp;12Trang / Page &amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>